<commit_message>
Added task for 1. user story.
</commit_message>
<xml_diff>
--- a/DraganMacura_Estimacija.xlsx
+++ b/DraganMacura_Estimacija.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Korisnik\OneDrive\SCH-Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VS19\TestProjekat\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
   <si>
     <t>Naziv taska</t>
   </si>
@@ -81,6 +81,30 @@
   </si>
   <si>
     <t>Estimacija</t>
+  </si>
+  <si>
+    <t>Dokerizacija</t>
+  </si>
+  <si>
+    <t>Kreiranje I konfiguracija MVC aplikacije</t>
+  </si>
+  <si>
+    <t>Implementacije integracije sa bankom</t>
+  </si>
+  <si>
+    <t>Kreiranje testova</t>
+  </si>
+  <si>
+    <t>Integracija servisnih metoda za User</t>
+  </si>
+  <si>
+    <t>Kreiranje intefejsa repositorijuma I implementacija repositorijuma za User</t>
+  </si>
+  <si>
+    <t>Kreiranje aplikativnih servisnih interfejsa I implementacija aplikativnih servisa za User</t>
+  </si>
+  <si>
+    <t>Kreiranje domenskih entiteta User I Transaction</t>
   </si>
 </sst>
 </file>
@@ -132,10 +156,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,21 +441,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="141.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -438,7 +463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -446,184 +471,270 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B8" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="2"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D38" s="2" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added rest of task and estimation for all tasks.
</commit_message>
<xml_diff>
--- a/DraganMacura_Estimacija.xlsx
+++ b/DraganMacura_Estimacija.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="36">
   <si>
     <t>Naziv taska</t>
   </si>
@@ -95,23 +95,50 @@
     <t>Kreiranje testova</t>
   </si>
   <si>
-    <t>Integracija servisnih metoda za User</t>
-  </si>
-  <si>
     <t>Kreiranje intefejsa repositorijuma I implementacija repositorijuma za User</t>
   </si>
   <si>
-    <t>Kreiranje aplikativnih servisnih interfejsa I implementacija aplikativnih servisa za User</t>
-  </si>
-  <si>
     <t>Kreiranje domenskih entiteta User I Transaction</t>
+  </si>
+  <si>
+    <t>Kreiranje intefejsa repositorijuma I implementacija repositorijuma za Transaction</t>
+  </si>
+  <si>
+    <t>Integracija servisnih metoda za User u MVC aplikaciji</t>
+  </si>
+  <si>
+    <t>Kreiranje intefejsa aplikativnih servisnih metoda I implementacija sa User</t>
+  </si>
+  <si>
+    <t>Kreiranje intefejsa aplikativnih servisnih metoda I implementacija sa Transaction</t>
+  </si>
+  <si>
+    <t>Dodavanje intefejsa za aplikativne servise I njihova implementacija</t>
+  </si>
+  <si>
+    <t>Integracija servisnih metoda u MVC aplikaciji</t>
+  </si>
+  <si>
+    <t>60min</t>
+  </si>
+  <si>
+    <t>30min</t>
+  </si>
+  <si>
+    <t>15min</t>
+  </si>
+  <si>
+    <t>120min</t>
+  </si>
+  <si>
+    <t>10min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +156,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -156,11 +190,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,6 +510,9 @@
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -494,49 +532,75 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="B12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="B13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="B14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="B16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="3"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -555,188 +619,463 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="A20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="3"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="A29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="3"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="4"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" s="4"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="3"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="3"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>29</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="4"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C46" s="3"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C47" s="3"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>29</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C51" s="4"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C52" s="3"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C53" s="3"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C56" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>29</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C57" s="4"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C58" s="3"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C59" s="3"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>29</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C63" s="4"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C64" s="3"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C65" s="3"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>29</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C69" s="4"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C70" s="3"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C71" s="3"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C74" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>2</v>
-      </c>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>29</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C75" s="1"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C76" s="1"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C77" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added real time for task.
</commit_message>
<xml_diff>
--- a/DraganMacura_Estimacija.xlsx
+++ b/DraganMacura_Estimacija.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="37">
   <si>
     <t>Naziv taska</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>10min</t>
+  </si>
+  <si>
+    <t>35min</t>
   </si>
 </sst>
 </file>
@@ -479,7 +482,7 @@
   <dimension ref="A1:C77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +540,9 @@
       <c r="B9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">

</xml_diff>

<commit_message>
Implemented service and repository.
</commit_message>
<xml_diff>
--- a/DraganMacura_Estimacija.xlsx
+++ b/DraganMacura_Estimacija.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="37">
   <si>
     <t>Naziv taska</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Integracija servisnih metoda za User u MVC aplikaciji</t>
   </si>
   <si>
-    <t>Kreiranje intefejsa aplikativnih servisnih metoda I implementacija sa User</t>
-  </si>
-  <si>
     <t>Kreiranje intefejsa aplikativnih servisnih metoda I implementacija sa Transaction</t>
   </si>
   <si>
@@ -135,6 +132,9 @@
   </si>
   <si>
     <t>35min</t>
+  </si>
+  <si>
+    <t>Kreiranje intefejsa aplikativnih servisnih metoda I implementacija za User</t>
   </si>
 </sst>
 </file>
@@ -482,7 +482,7 @@
   <dimension ref="A1:C77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,7 +514,7 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -538,36 +538,40 @@
         <v>24</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" s="3"/>
     </row>
@@ -576,7 +580,7 @@
         <v>19</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="3"/>
     </row>
@@ -585,7 +589,7 @@
         <v>20</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="3"/>
     </row>
@@ -594,7 +598,7 @@
         <v>26</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="3"/>
     </row>
@@ -603,7 +607,7 @@
         <v>22</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="3"/>
     </row>
@@ -625,10 +629,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" s="3"/>
     </row>
@@ -637,16 +641,16 @@
         <v>25</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" s="3"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="3"/>
     </row>
@@ -655,7 +659,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" s="3"/>
     </row>
@@ -681,19 +685,19 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27" s="3"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" s="3"/>
     </row>
@@ -702,7 +706,7 @@
         <v>22</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C29" s="3"/>
     </row>
@@ -728,19 +732,19 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C33" s="4"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C34" s="3"/>
     </row>
@@ -749,7 +753,7 @@
         <v>22</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C35" s="3"/>
     </row>
@@ -775,19 +779,19 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C39" s="4"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C40" s="3"/>
     </row>
@@ -796,7 +800,7 @@
         <v>22</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C41" s="3"/>
     </row>
@@ -822,19 +826,19 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C45" s="4"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C46" s="3"/>
     </row>
@@ -843,7 +847,7 @@
         <v>22</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C47" s="3"/>
     </row>
@@ -869,19 +873,19 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C51" s="4"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C52" s="3"/>
     </row>
@@ -890,7 +894,7 @@
         <v>22</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C53" s="3"/>
     </row>
@@ -916,19 +920,19 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C57" s="4"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C58" s="3"/>
     </row>
@@ -937,7 +941,7 @@
         <v>22</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C59" s="3"/>
     </row>
@@ -963,19 +967,19 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C63" s="4"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C64" s="3"/>
     </row>
@@ -984,7 +988,7 @@
         <v>22</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C65" s="3"/>
     </row>
@@ -1010,19 +1014,19 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C69" s="4"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C70" s="3"/>
     </row>
@@ -1031,7 +1035,7 @@
         <v>22</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C71" s="3"/>
     </row>
@@ -1057,19 +1061,19 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C75" s="1"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C76" s="1"/>
     </row>
@@ -1078,7 +1082,7 @@
         <v>22</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C77" s="1"/>
     </row>

</xml_diff>

<commit_message>
Added mvc application and implemented user usecase.
</commit_message>
<xml_diff>
--- a/DraganMacura_Estimacija.xlsx
+++ b/DraganMacura_Estimacija.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="39">
   <si>
     <t>Naziv taska</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>Kreiranje intefejsa aplikativnih servisnih metoda I implementacija za User</t>
+  </si>
+  <si>
+    <t>Konfigurisanje EF</t>
+  </si>
+  <si>
+    <t>50min</t>
   </si>
 </sst>
 </file>
@@ -479,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,77 +574,87 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="C17" s="3"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>32</v>
@@ -647,430 +663,430 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C22" s="3"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="3"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="3"/>
+      <c r="B24" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C24" s="3"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="3"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="B28" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C28" s="3"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="3"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="3"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="3"/>
+      <c r="B30" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C30" s="3"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" s="4"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="B34" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="C34" s="4"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" s="3"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="3"/>
+      <c r="B36" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C36" s="3"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>28</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="4"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C40" s="3"/>
+      <c r="C40" s="4"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41" s="3"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C41" s="3"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="3"/>
+      <c r="B42" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C42" s="3"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>28</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B46" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C45" s="4"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C46" s="3"/>
+      <c r="C46" s="4"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C47" s="3"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C47" s="3"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B48" s="3"/>
+      <c r="B48" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C48" s="3"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>28</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B52" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C51" s="4"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C52" s="3"/>
+      <c r="C52" s="4"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C53" s="3"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B53" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C53" s="3"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B54" s="3"/>
+      <c r="B54" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C54" s="3"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>28</v>
       </c>
-      <c r="B57" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C57" s="4"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="B58" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C58" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="C58" s="4"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C59" s="3"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C59" s="3"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="3"/>
+      <c r="B60" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C60" s="3"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B63" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C63" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>28</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B64" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C63" s="4"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C64" s="3"/>
+      <c r="C64" s="4"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C65" s="3"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B65" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C65" s="3"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B66" s="3"/>
+      <c r="B66" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C66" s="3"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C69" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>28</v>
       </c>
-      <c r="B69" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C69" s="4"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="B70" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C70" s="3"/>
+      <c r="C70" s="4"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C71" s="3"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B71" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C71" s="3"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B72" s="3"/>
+      <c r="B72" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C72" s="3"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C75" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>28</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C75" s="1"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>31</v>
@@ -1079,12 +1095,21 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C77" s="1"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B77" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C77" s="1"/>
+      <c r="B78" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C78" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changed time for estimation.
</commit_message>
<xml_diff>
--- a/DraganMacura_Estimacija.xlsx
+++ b/DraganMacura_Estimacija.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="39">
   <si>
     <t>Naziv taska</t>
   </si>
@@ -488,7 +488,7 @@
   <dimension ref="A1:C78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,7 +634,9 @@
       <c r="B17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">

</xml_diff>

<commit_message>
Implemented transaction service in the mvc application.
</commit_message>
<xml_diff>
--- a/DraganMacura_Estimacija.xlsx
+++ b/DraganMacura_Estimacija.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="42">
   <si>
     <t>Naziv taska</t>
   </si>
@@ -141,6 +141,15 @@
   </si>
   <si>
     <t>50min</t>
+  </si>
+  <si>
+    <t>Dopuna transation entiteta</t>
+  </si>
+  <si>
+    <t>Konfiguracija EF</t>
+  </si>
+  <si>
+    <t>40min</t>
   </si>
 </sst>
 </file>
@@ -485,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:C80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,462 +665,490 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="3"/>
+      <c r="C22" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="3"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="B26" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" s="3"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="B30" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="3"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="B31" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="3"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="B32" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="3"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34" s="4"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="B36" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="4"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="3"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="B37" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C36" s="3"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="B38" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="3"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="4"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="C42" s="4"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C41" s="3"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="B43" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" s="3"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C42" s="3"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="B44" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C44" s="3"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>28</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B48" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C46" s="4"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+      <c r="C48" s="4"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C47" s="3"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="B49" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C49" s="3"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C48" s="3"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="B50" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C50" s="3"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>28</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B54" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C52" s="4"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+      <c r="C54" s="4"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B53" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C53" s="3"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
+      <c r="B55" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C55" s="3"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C54" s="3"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+      <c r="B56" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C56" s="3"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C59" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>28</v>
       </c>
-      <c r="B58" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C58" s="4"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
+      <c r="B60" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C60" s="4"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C59" s="3"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
+      <c r="B61" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C61" s="3"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B60" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C60" s="3"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+      <c r="B62" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C62" s="3"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C65" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>28</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B66" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C64" s="4"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
+      <c r="C66" s="4"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B65" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C65" s="3"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
+      <c r="B67" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C67" s="3"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B66" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C66" s="3"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+      <c r="B68" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C68" s="3"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C71" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>28</v>
       </c>
-      <c r="B70" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C70" s="4"/>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
+      <c r="B72" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C72" s="4"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B71" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C71" s="3"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
+      <c r="B73" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C73" s="3"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B72" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C72" s="3"/>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+      <c r="B74" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C74" s="3"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C77" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>28</v>
       </c>
-      <c r="B76" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C76" s="1"/>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
+      <c r="B78" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C78" s="1"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B77" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C77" s="1"/>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
+      <c r="B79" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C79" s="1"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B78" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C78" s="1"/>
+      <c r="B80" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C80" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implemented usecase for bank withdraw.
</commit_message>
<xml_diff>
--- a/DraganMacura_Estimacija.xlsx
+++ b/DraganMacura_Estimacija.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="43">
   <si>
     <t>Naziv taska</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>40min</t>
+  </si>
+  <si>
+    <t>5min</t>
   </si>
 </sst>
 </file>
@@ -496,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,7 +759,9 @@
       <c r="B30" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="3"/>
+      <c r="C30" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
@@ -765,7 +770,9 @@
       <c r="B31" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="3"/>
+      <c r="C31" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
@@ -774,7 +781,9 @@
       <c r="B32" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="3"/>
+      <c r="C32" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B33" s="3"/>

</xml_diff>

<commit_message>
Implemented users transaction in the mvc application.
</commit_message>
<xml_diff>
--- a/DraganMacura_Estimacija.xlsx
+++ b/DraganMacura_Estimacija.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="43">
   <si>
     <t>Naziv taska</t>
   </si>
@@ -500,7 +500,7 @@
   <dimension ref="A1:C80"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,7 +812,9 @@
       <c r="B36" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="4"/>
+      <c r="C36" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">

</xml_diff>

<commit_message>
Added change user pass.
</commit_message>
<xml_diff>
--- a/DraganMacura_Estimacija.xlsx
+++ b/DraganMacura_Estimacija.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="43">
   <si>
     <t>Naziv taska</t>
   </si>
@@ -499,7 +499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
       <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
@@ -1018,7 +1018,9 @@
       <c r="B60" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C60" s="4"/>
+      <c r="C60" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
@@ -1027,7 +1029,9 @@
       <c r="B61" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C61" s="3"/>
+      <c r="C61" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
@@ -1036,7 +1040,9 @@
       <c r="B62" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C62" s="3"/>
+      <c r="C62" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B63" s="3"/>
@@ -1134,7 +1140,9 @@
       <c r="B74" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C74" s="3"/>
+      <c r="C74" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B75" s="3"/>

</xml_diff>

<commit_message>
Added block and unblock action for user.
</commit_message>
<xml_diff>
--- a/DraganMacura_Estimacija.xlsx
+++ b/DraganMacura_Estimacija.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="43">
   <si>
     <t>Naziv taska</t>
   </si>
@@ -499,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,7 +918,9 @@
       <c r="B48" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C48" s="4"/>
+      <c r="C48" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
@@ -927,7 +929,9 @@
       <c r="B49" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C49" s="3"/>
+      <c r="C49" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
@@ -936,7 +940,9 @@
       <c r="B50" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C50" s="3"/>
+      <c r="C50" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B51" s="3"/>
@@ -1071,7 +1077,9 @@
       <c r="B66" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C66" s="4"/>
+      <c r="C66" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
@@ -1080,7 +1088,9 @@
       <c r="B67" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C67" s="3"/>
+      <c r="C67" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
@@ -1089,7 +1099,9 @@
       <c r="B68" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C68" s="3"/>
+      <c r="C68" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B69" s="3"/>

</xml_diff>

<commit_message>
Added month limit per user.
</commit_message>
<xml_diff>
--- a/DraganMacura_Estimacija.xlsx
+++ b/DraganMacura_Estimacija.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="43">
   <si>
     <t>Naziv taska</t>
   </si>
@@ -499,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78:C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1183,7 +1183,9 @@
       <c r="B78" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C78" s="1"/>
+      <c r="C78" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
@@ -1192,7 +1194,9 @@
       <c r="B79" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C79" s="1"/>
+      <c r="C79" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
@@ -1201,7 +1205,9 @@
       <c r="B80" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C80" s="1"/>
+      <c r="C80" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>